<commit_message>
Upload latest single-day multi-day output to Dropbox
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-09-28.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-09-28.xlsx
@@ -555,16 +555,16 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44101</v>
+        <v>44102</v>
       </c>
       <c r="C4" t="n">
-        <v>86269</v>
+        <v>86638</v>
       </c>
       <c r="D4" t="n">
         <v>2100</v>
       </c>
       <c r="E4" t="n">
-        <v>3474</v>
+        <v>3487</v>
       </c>
       <c r="F4" t="n">
         <v>66</v>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>58859</v>
+        <v>59093</v>
       </c>
       <c r="L4" t="n">
         <v>2095</v>

</xml_diff>